<commit_message>
- Add test template data; - Update test xlsx data;
</commit_message>
<xml_diff>
--- a/test/data/test.xlsx
+++ b/test/data/test.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>!</t>
   </si>
@@ -35,6 +35,12 @@
   </si>
   <si>
     <t>value</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>max</t>
   </si>
   <si>
     <t>desc</t>
@@ -208,15 +214,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="16.9073170731707"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="18.2"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -226,6 +232,8 @@
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
@@ -240,11 +248,17 @@
       <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="0" t="s">
-        <v>5</v>
+      <c r="H2" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -253,17 +267,23 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="1" t="n">
+        <v>123</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="G3" s="0" t="n">
         <f aca="false">D3/100</f>
         <v>1</v>
       </c>
-      <c r="F3" s="0" t="s">
-        <v>7</v>
+      <c r="H3" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -272,17 +292,23 @@
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>200</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="1" t="n">
+        <v>321</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="G4" s="0" t="n">
         <f aca="false">D4/100</f>
         <v>2</v>
       </c>
-      <c r="F4" s="0" t="s">
-        <v>9</v>
+      <c r="H4" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -290,17 +316,23 @@
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>300</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5" s="1" t="n">
+        <v>456</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>99</v>
+      </c>
+      <c r="G5" s="0" t="n">
         <f aca="false">D5/100</f>
         <v>3</v>
       </c>
-      <c r="F5" s="0" t="s">
-        <v>11</v>
+      <c r="H5" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -308,17 +340,23 @@
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>400</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6" s="1" t="n">
+        <v>4895</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="G6" s="0" t="n">
         <f aca="false">D6/100</f>
         <v>4</v>
       </c>
-      <c r="F6" s="0" t="s">
-        <v>13</v>
+      <c r="H6" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -326,17 +364,23 @@
         <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>500</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E7" s="1" t="n">
+        <v>21546</v>
+      </c>
+      <c r="F7" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="G7" s="0" t="n">
         <f aca="false">D7/100</f>
         <v>5</v>
       </c>
-      <c r="F7" s="0" t="s">
-        <v>15</v>
+      <c r="H7" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -344,17 +388,23 @@
         <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>600</v>
       </c>
-      <c r="E8" s="0" t="n">
+      <c r="E8" s="1" t="n">
+        <v>45.54</v>
+      </c>
+      <c r="F8" s="1" t="n">
+        <v>99</v>
+      </c>
+      <c r="G8" s="0" t="n">
         <f aca="false">D8/100</f>
         <v>6</v>
       </c>
-      <c r="F8" s="0" t="s">
-        <v>17</v>
+      <c r="H8" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -362,17 +412,23 @@
         <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>700</v>
       </c>
-      <c r="E9" s="0" t="n">
+      <c r="E9" s="1" t="n">
+        <v>453.54</v>
+      </c>
+      <c r="F9" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="G9" s="0" t="n">
         <f aca="false">D9/100</f>
         <v>7</v>
       </c>
-      <c r="F9" s="0" t="s">
-        <v>19</v>
+      <c r="H9" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -380,17 +436,23 @@
         <v>8</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>800</v>
       </c>
-      <c r="E10" s="0" t="n">
+      <c r="E10" s="1" t="n">
+        <v>5.9</v>
+      </c>
+      <c r="F10" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="G10" s="0" t="n">
         <f aca="false">D10/100</f>
         <v>8</v>
       </c>
-      <c r="F10" s="0" t="s">
-        <v>21</v>
+      <c r="H10" s="0" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -398,17 +460,23 @@
         <v>9</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D11" s="1" t="n">
         <v>900</v>
       </c>
-      <c r="E11" s="0" t="n">
+      <c r="E11" s="1" t="n">
+        <v>9.99</v>
+      </c>
+      <c r="F11" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="G11" s="0" t="n">
         <f aca="false">D11/100</f>
         <v>9</v>
       </c>
-      <c r="F11" s="0" t="s">
-        <v>23</v>
+      <c r="H11" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -416,17 +484,23 @@
         <v>10</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D12" s="1" t="n">
         <v>1000</v>
       </c>
-      <c r="E12" s="0" t="n">
+      <c r="E12" s="1" t="n">
+        <v>1003.5</v>
+      </c>
+      <c r="F12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G12" s="0" t="n">
         <f aca="false">D12/100</f>
         <v>10</v>
       </c>
-      <c r="F12" s="0" t="s">
-        <v>25</v>
+      <c r="H12" s="0" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Update the test data;
</commit_message>
<xml_diff>
--- a/test/data/test.xlsx
+++ b/test/data/test.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="demo" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="test" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
   <si>
     <t>!</t>
   </si>
@@ -104,6 +105,27 @@
   </si>
   <si>
     <t>desc10</t>
+  </si>
+  <si>
+    <t>Della</t>
+  </si>
+  <si>
+    <t>Neka</t>
+  </si>
+  <si>
+    <t>Ares</t>
+  </si>
+  <si>
+    <t>Lome</t>
+  </si>
+  <si>
+    <t>Chopper</t>
+  </si>
+  <si>
+    <t>Spy</t>
+  </si>
+  <si>
+    <t>Wolly</t>
   </si>
 </sst>
 </file>
@@ -216,13 +238,13 @@
   </sheetPr>
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="18.2"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="19.619512195122"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -512,4 +534,210 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G9"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1" t="n">
+        <v>234234</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="E3" s="1" t="n">
+        <v>123</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <f aca="false">D3/100</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1" t="n">
+        <v>4582</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>321</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <f aca="false">D4/100</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="1" t="n">
+        <v>45672</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>300</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>456</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>99</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <f aca="false">D5/100</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="1" t="n">
+        <v>5428</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>400</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <v>4895</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <f aca="false">D6/100</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>500</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <v>21546</v>
+      </c>
+      <c r="F7" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <f aca="false">D7/100</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="1" t="n">
+        <v>62654</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>600</v>
+      </c>
+      <c r="E8" s="1" t="n">
+        <v>45.54</v>
+      </c>
+      <c r="F8" s="1" t="n">
+        <v>99</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <f aca="false">D8/100</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="1" t="n">
+        <v>943452</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>700</v>
+      </c>
+      <c r="E9" s="1" t="n">
+        <v>453.54</v>
+      </c>
+      <c r="F9" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <f aca="false">D9/100</f>
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,標準"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,標準"&amp;12頁 &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
- update test data;
</commit_message>
<xml_diff>
--- a/test/data/test.xlsx
+++ b/test/data/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="demo" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="41">
   <si>
     <t>!</t>
   </si>
@@ -142,6 +142,9 @@
   </si>
   <si>
     <t>1.0.0</t>
+  </si>
+  <si>
+    <t>newname</t>
   </si>
 </sst>
 </file>
@@ -269,7 +272,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="24.5219512195122"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="26.4585365853658"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -571,13 +574,13 @@
   </sheetPr>
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.5853658536585"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3560975609756"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -783,13 +786,13 @@
   </sheetPr>
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.93658536585366"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.5853658536585"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -805,8 +808,15 @@
       <c r="D1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
+      <c r="E1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">

</xml_diff>

<commit_message>
Updated the test file. Add new tag to test.
</commit_message>
<xml_diff>
--- a/test/data/test.xlsx
+++ b/test/data/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="test" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,99 +20,105 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
-  <si>
-    <t>!</t>
-  </si>
-  <si>
-    <t>^</t>
-  </si>
-  <si>
-    <t>version</t>
-  </si>
-  <si>
-    <t>1.0.0</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>newname</t>
-  </si>
-  <si>
-    <t>#</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>value</t>
-  </si>
-  <si>
-    <t>Id_1</t>
-  </si>
-  <si>
-    <t>Della</t>
-  </si>
-  <si>
-    <t>ignore</t>
-  </si>
-  <si>
-    <t>Value_1</t>
-  </si>
-  <si>
-    <t>Id_2</t>
-  </si>
-  <si>
-    <t>Neka</t>
-  </si>
-  <si>
-    <t>Value_2</t>
-  </si>
-  <si>
-    <t>Id_3</t>
-  </si>
-  <si>
-    <t>Ares</t>
-  </si>
-  <si>
-    <t>Value_3</t>
-  </si>
-  <si>
-    <t>Id_4</t>
-  </si>
-  <si>
-    <t>Lome</t>
-  </si>
-  <si>
-    <t>Value_4</t>
-  </si>
-  <si>
-    <t>Id_5</t>
-  </si>
-  <si>
-    <t>Chopper</t>
-  </si>
-  <si>
-    <t>Value_5</t>
-  </si>
-  <si>
-    <t>Id_6</t>
-  </si>
-  <si>
-    <t>Spy</t>
-  </si>
-  <si>
-    <t>Value_6</t>
-  </si>
-  <si>
-    <t>Id_7</t>
-  </si>
-  <si>
-    <t>Wolly</t>
-  </si>
-  <si>
-    <t>Value_7</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
+  <si>
+    <t xml:space="preserve">!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">^</t>
+  </si>
+  <si>
+    <t xml:space="preserve">version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.0.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">~</t>
+  </si>
+  <si>
+    <t xml:space="preserve">items</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Id_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Della</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ignore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Id_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Neka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Id_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ares</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Id_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Id_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chopper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Id_6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value_6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Id_7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wolly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value_7</t>
   </si>
 </sst>
 </file>
@@ -120,7 +126,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="5">
@@ -135,16 +141,19 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="136"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="136"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="136"/>
     </font>
     <font>
       <sz val="10"/>
@@ -225,15 +234,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
+      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.2292682926829"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -258,13 +267,19 @@
       <c r="G1" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="H1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>4</v>
@@ -273,104 +288,104 @@
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -378,8 +393,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12頁 &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,標準"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,標準"&amp;12頁 &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>